<commit_message>
Added alternatives for amplification to the parts list
</commit_message>
<xml_diff>
--- a/Parts List.xlsx
+++ b/Parts List.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwprod-my.sharepoint.com/personal/sanwalka_wisc_edu/Documents/WHAM/Circuits/Charge Sensitive Amplifier/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwprod-my.sharepoint.com/personal/sanwalka_wisc_edu/Documents/WHAM/Circuits/Charge Sensitive Amplifier Rev. 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="440" documentId="8_{0EBB8B5F-FC1B-4E3D-BBF1-B0CA844F24E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA4E0B50-6904-4A08-8F80-4AB9FF85F772}"/>
+  <xr:revisionPtr revIDLastSave="481" documentId="8_{0EBB8B5F-FC1B-4E3D-BBF1-B0CA844F24E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3CB3970-D546-499B-80E2-B2B0FD64E623}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{86E9DEB7-43CD-4D23-8FD0-DFC98C177167}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{86E9DEB7-43CD-4D23-8FD0-DFC98C177167}"/>
   </bookViews>
   <sheets>
     <sheet name="By part number" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="115">
   <si>
     <t>Part Number</t>
   </si>
@@ -283,9 +283,6 @@
     <t>471-SMARACONNECTOR</t>
   </si>
   <si>
-    <t>IC1</t>
-  </si>
-  <si>
     <t>IC2</t>
   </si>
   <si>
@@ -359,6 +356,30 @@
   </si>
   <si>
     <t>863-MC78M05ACDTRKG</t>
+  </si>
+  <si>
+    <t>See below</t>
+  </si>
+  <si>
+    <t>R11 other options</t>
+  </si>
+  <si>
+    <t>IC5</t>
+  </si>
+  <si>
+    <t>0 Ohm resistor</t>
+  </si>
+  <si>
+    <t>652-CR1206-J/-000ELF</t>
+  </si>
+  <si>
+    <t>652-CR1206FX-2000ELF</t>
+  </si>
+  <si>
+    <t>Thin Film</t>
+  </si>
+  <si>
+    <t>71-PTN1206Y5000BST1</t>
   </si>
 </sst>
 </file>
@@ -742,16 +763,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E528EE5B-7B78-46FF-B994-150BC36B17B6}">
-  <dimension ref="A1:G66"/>
+  <dimension ref="A1:H73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G78" sqref="G78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="11.234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.234375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.9375" style="3"/>
     <col min="3" max="3" width="14.29296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.234375" bestFit="1" customWidth="1"/>
@@ -779,7 +800,7 @@
         <v>53</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.5">
@@ -1027,13 +1048,13 @@
         <v>15</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D14" t="s">
         <v>46</v>
       </c>
       <c r="G14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.5">
@@ -1096,7 +1117,7 @@
         <v>0.1</v>
       </c>
       <c r="G17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.5">
@@ -1124,13 +1145,13 @@
         <v>20</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D19" t="s">
         <v>46</v>
       </c>
       <c r="G19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.5">
@@ -1173,7 +1194,7 @@
         <v>0.1</v>
       </c>
       <c r="G21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.5">
@@ -1181,13 +1202,13 @@
         <v>23</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D22" t="s">
         <v>46</v>
       </c>
       <c r="G22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.5">
@@ -1215,13 +1236,13 @@
         <v>25</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D24" t="s">
         <v>46</v>
       </c>
       <c r="G24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.5">
@@ -1264,7 +1285,7 @@
         <v>0.1</v>
       </c>
       <c r="G26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.5">
@@ -1272,13 +1293,13 @@
         <v>28</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D27" t="s">
         <v>46</v>
       </c>
       <c r="G27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.5">
@@ -1301,47 +1322,47 @@
         <v>0.1</v>
       </c>
       <c r="G28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29" t="s">
         <v>98</v>
-      </c>
-      <c r="C29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D29" t="s">
-        <v>46</v>
-      </c>
-      <c r="E29" t="s">
-        <v>99</v>
       </c>
       <c r="F29">
         <v>0.37</v>
       </c>
       <c r="G29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" t="s">
+        <v>46</v>
+      </c>
+      <c r="E30" t="s">
         <v>98</v>
-      </c>
-      <c r="C30" t="s">
-        <v>48</v>
-      </c>
-      <c r="D30" t="s">
-        <v>46</v>
-      </c>
-      <c r="E30" t="s">
-        <v>99</v>
       </c>
       <c r="F30">
         <v>0.37</v>
@@ -1349,25 +1370,25 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="C31" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31" t="s">
         <v>98</v>
-      </c>
-      <c r="C31" t="s">
-        <v>48</v>
-      </c>
-      <c r="D31" t="s">
-        <v>46</v>
-      </c>
-      <c r="E31" t="s">
-        <v>99</v>
       </c>
       <c r="F31">
         <v>0.37</v>
       </c>
       <c r="G31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.5">
@@ -1390,7 +1411,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1410,35 +1431,35 @@
         <v>3.66</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
         <v>32</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D34" t="s">
         <v>46</v>
       </c>
       <c r="G34" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.5">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
         <v>33</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D35" t="s">
         <v>46</v>
       </c>
       <c r="G35" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.5">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1458,21 +1479,21 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A37" t="s">
         <v>35</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D37" t="s">
         <v>46</v>
       </c>
       <c r="G37" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.5">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1492,10 +1513,10 @@
         <v>0.27</v>
       </c>
       <c r="G38" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.5">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1509,46 +1530,46 @@
         <v>46</v>
       </c>
       <c r="E39" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F39">
         <v>0.27</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A40" t="s">
         <v>38</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D40" t="s">
         <v>46</v>
       </c>
       <c r="G40" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.5">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A41" t="s">
         <v>39</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D41" t="s">
         <v>46</v>
       </c>
       <c r="G41" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.5">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A42" t="s">
         <v>40</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C42" t="s">
         <v>69</v>
@@ -1557,41 +1578,44 @@
         <v>46</v>
       </c>
       <c r="E42" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F42">
         <v>0.38</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H42" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A43" t="s">
         <v>41</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D43" t="s">
         <v>46</v>
       </c>
       <c r="G43" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.5">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A44" t="s">
         <v>42</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
       </c>
       <c r="G44" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.5">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -1611,7 +1635,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -1631,40 +1655,40 @@
         <v>0.16</v>
       </c>
       <c r="G46" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.5">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A47" t="s">
+        <v>99</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D47" t="s">
+        <v>46</v>
+      </c>
+      <c r="G47" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A48" t="s">
         <v>100</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D47" t="s">
-        <v>46</v>
-      </c>
-      <c r="G47" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A48" t="s">
+      <c r="B48" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>102</v>
-      </c>
       <c r="D48" t="s">
         <v>46</v>
       </c>
       <c r="G48" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A49" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>74</v>
@@ -1682,21 +1706,21 @@
         <v>0.27</v>
       </c>
       <c r="G49" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A50" t="s">
+        <v>89</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="D50" t="s">
+        <v>46</v>
+      </c>
+      <c r="E50" t="s">
         <v>91</v>
-      </c>
-      <c r="D50" t="s">
-        <v>46</v>
-      </c>
-      <c r="E50" t="s">
-        <v>92</v>
       </c>
       <c r="F50">
         <v>1.54</v>
@@ -1753,7 +1777,7 @@
         <v>1.7</v>
       </c>
       <c r="G53" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.5">
@@ -1784,7 +1808,7 @@
         <v>46</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F55">
         <v>0.61</v>
@@ -1798,7 +1822,7 @@
         <v>46</v>
       </c>
       <c r="E56" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F56">
         <v>14.47</v>
@@ -1812,10 +1836,13 @@
         <v>46</v>
       </c>
       <c r="E57" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F57">
         <v>14.47</v>
+      </c>
+      <c r="G57" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.5">
@@ -1826,7 +1853,7 @@
         <v>46</v>
       </c>
       <c r="E58" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F58">
         <v>14.47</v>
@@ -1834,39 +1861,116 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A59" t="s">
+        <v>109</v>
+      </c>
+      <c r="D59" t="s">
+        <v>46</v>
+      </c>
+      <c r="E59" t="s">
         <v>85</v>
-      </c>
-      <c r="D59" t="s">
-        <v>46</v>
-      </c>
-      <c r="E59" t="s">
-        <v>86</v>
       </c>
       <c r="F59">
         <v>14.47</v>
       </c>
+      <c r="G59" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A60" t="s">
+        <v>86</v>
+      </c>
+      <c r="D60" t="s">
         <v>87</v>
       </c>
-      <c r="D60" t="s">
+      <c r="E60" t="s">
         <v>88</v>
-      </c>
-      <c r="E60" t="s">
-        <v>89</v>
       </c>
       <c r="F60">
         <v>22.67</v>
       </c>
     </row>
-    <row r="66" spans="5:6" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.5">
       <c r="E66" t="s">
         <v>73</v>
       </c>
       <c r="F66">
         <f>SUM(F2:F65)</f>
         <v>100.37</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A69" t="s">
+        <v>108</v>
+      </c>
+      <c r="B69" s="3">
+        <v>500</v>
+      </c>
+      <c r="C69" t="s">
+        <v>113</v>
+      </c>
+      <c r="D69" t="s">
+        <v>46</v>
+      </c>
+      <c r="E69" t="s">
+        <v>114</v>
+      </c>
+      <c r="F69">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="B70" s="3">
+        <v>200</v>
+      </c>
+      <c r="C70" t="s">
+        <v>69</v>
+      </c>
+      <c r="D70" t="s">
+        <v>46</v>
+      </c>
+      <c r="E70" t="s">
+        <v>112</v>
+      </c>
+      <c r="F70">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="B71" s="3">
+        <v>100</v>
+      </c>
+      <c r="C71" t="s">
+        <v>69</v>
+      </c>
+      <c r="D71" t="s">
+        <v>46</v>
+      </c>
+      <c r="E71" t="s">
+        <v>104</v>
+      </c>
+      <c r="F71">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A73" t="s">
+        <v>110</v>
+      </c>
+      <c r="B73" s="3">
+        <v>0</v>
+      </c>
+      <c r="C73" t="s">
+        <v>69</v>
+      </c>
+      <c r="D73" t="s">
+        <v>46</v>
+      </c>
+      <c r="E73" t="s">
+        <v>111</v>
+      </c>
+      <c r="F73">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added alternatives for the feedback resistor for the 1st stage
</commit_message>
<xml_diff>
--- a/Parts List.xlsx
+++ b/Parts List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwprod-my.sharepoint.com/personal/sanwalka_wisc_edu/Documents/WHAM/Circuits/Charge Sensitive Amplifier Rev. 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="481" documentId="8_{0EBB8B5F-FC1B-4E3D-BBF1-B0CA844F24E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3CB3970-D546-499B-80E2-B2B0FD64E623}"/>
+  <xr:revisionPtr revIDLastSave="495" documentId="8_{0EBB8B5F-FC1B-4E3D-BBF1-B0CA844F24E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1FC96BE3-37DE-4442-ADBA-652E2FB5B650}"/>
   <bookViews>
     <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{86E9DEB7-43CD-4D23-8FD0-DFC98C177167}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="121">
   <si>
     <t>Part Number</t>
   </si>
@@ -380,6 +380,24 @@
   </si>
   <si>
     <t>71-PTN1206Y5000BST1</t>
+  </si>
+  <si>
+    <t>R5 other options</t>
+  </si>
+  <si>
+    <t>50M</t>
+  </si>
+  <si>
+    <t>5M</t>
+  </si>
+  <si>
+    <t>71-CRHA1206A50M0FKEF</t>
+  </si>
+  <si>
+    <t>652-CHV1206FX1005ELF</t>
+  </si>
+  <si>
+    <t>588-HVC1206T5004JET</t>
   </si>
 </sst>
 </file>
@@ -763,11 +781,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E528EE5B-7B78-46FF-B994-150BC36B17B6}">
-  <dimension ref="A1:H73"/>
+  <dimension ref="A1:H77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G78" sqref="G78"/>
+      <selection pane="bottomLeft" activeCell="K71" sqref="K71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1478,6 +1496,9 @@
       <c r="F36">
         <v>0.69</v>
       </c>
+      <c r="H36" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A37" t="s">
@@ -1955,10 +1976,10 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A73" t="s">
-        <v>110</v>
-      </c>
-      <c r="B73" s="3">
-        <v>0</v>
+        <v>115</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="C73" t="s">
         <v>69</v>
@@ -1967,9 +1988,63 @@
         <v>46</v>
       </c>
       <c r="E73" t="s">
+        <v>118</v>
+      </c>
+      <c r="F73">
+        <v>1.85</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="B74" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C74" t="s">
+        <v>69</v>
+      </c>
+      <c r="D74" t="s">
+        <v>46</v>
+      </c>
+      <c r="E74" t="s">
+        <v>119</v>
+      </c>
+      <c r="F74">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="B75" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C75" t="s">
+        <v>69</v>
+      </c>
+      <c r="D75" t="s">
+        <v>46</v>
+      </c>
+      <c r="E75" t="s">
+        <v>120</v>
+      </c>
+      <c r="F75">
+        <v>1.89</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A77" t="s">
+        <v>110</v>
+      </c>
+      <c r="B77" s="3">
+        <v>0</v>
+      </c>
+      <c r="C77" t="s">
+        <v>69</v>
+      </c>
+      <c r="D77" t="s">
+        <v>46</v>
+      </c>
+      <c r="E77" t="s">
         <v>111</v>
       </c>
-      <c r="F73">
+      <c r="F77">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>